<commit_message>
ASKAPSDP-2214 work in progress on component ingest
</commit_message>
<xml_diff>
--- a/Code/Components/Services/skymodel/current/schema_definitions/GSM_casda_polarisation.xlsx
+++ b/Code/Components/Services/skymodel/current/schema_definitions/GSM_casda_polarisation.xlsx
@@ -31,8 +31,7 @@
             <family val="2"/>
             <charset val="1"/>
           </rPr>
-          <t>Author:
-</t>
+          <t>Author:</t>
         </r>
         <r>
           <rPr>
@@ -51,7 +50,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="207" uniqueCount="135">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="211" uniqueCount="139">
   <si>
     <t>gsm.polarisation_component 
 10 November 2016</t>
@@ -99,6 +98,18 @@
     <t>Not required. Stored in component table</t>
   </si>
   <si>
+    <t>component_id</t>
+  </si>
+  <si>
+    <t>meta.id;meta.main</t>
+  </si>
+  <si>
+    <t>Component identifier</t>
+  </si>
+  <si>
+    <t>VARCHAR</t>
+  </si>
+  <si>
     <t>ra_deg_cont</t>
   </si>
   <si>
@@ -222,7 +233,7 @@
     <t>co_4</t>
   </si>
   <si>
-    <t>Fourth order coefficient for polynomial fit to Stokes I spectrum </t>
+    <t>Fourth order coefficient for polynomial fit to Stokes I spectrum</t>
   </si>
   <si>
     <t>co_5</t>
@@ -270,7 +281,7 @@
     <t>phot.flux.density;phys.polarization.rotMeasure;stat.max;askap:meta.corrected</t>
   </si>
   <si>
-    <t>Effective peak polarised intensity after correction for bias </t>
+    <t>Effective peak polarised intensity after correction for bias</t>
   </si>
   <si>
     <t>pol_peak_err</t>
@@ -288,7 +299,7 @@
     <t>phot.flux.density;phys.polarization.rotMeasure;stat.max;stat.fit</t>
   </si>
   <si>
-    <t>Peak polarised intensity from a three-point parabolic fit </t>
+    <t>Peak polarised intensity from a three-point parabolic fit</t>
   </si>
   <si>
     <t>pol_peak_fit_debias</t>
@@ -297,7 +308,7 @@
     <t>phot.flux.density;phys.polarization.rotMeasure;stat.max;stat.fit;askap:meta.corrected</t>
   </si>
   <si>
-    <t>Peak polarised intensity, corrected for bias, from a three-point parabolic fit </t>
+    <t>Peak polarised intensity, corrected for bias, from a three-point parabolic fit</t>
   </si>
   <si>
     <t>pol_peak_fit_err</t>
@@ -306,7 +317,7 @@
     <t>stat.error;phot.flux.density;phys.polarization.rotMeasure;stat.max;stat.fit</t>
   </si>
   <si>
-    <t>Uncertainty in pol_peak_fit </t>
+    <t>Uncertainty in pol_peak_fit</t>
   </si>
   <si>
     <t>pol_peak_fit_snr</t>
@@ -330,7 +341,7 @@
     <t>fd_peak</t>
   </si>
   <si>
-    <t>phys.polarization.rotMeasure </t>
+    <t>phys.polarization.rotMeasure</t>
   </si>
   <si>
     <t>Faraday Depth from the channel with the peak of the Faraday Dispersion Function</t>
@@ -339,7 +350,7 @@
     <t>fd_peak_err</t>
   </si>
   <si>
-    <t>stat.error;phys.polarization.rotMeasure </t>
+    <t>stat.error;phys.polarization.rotMeasure</t>
   </si>
   <si>
     <t>Uncertainty in far_depth_peak</t>
@@ -429,7 +440,7 @@
     <t>complex_2</t>
   </si>
   <si>
-    <t>Statistical measure of polarisation complexity after removal of a thin-screen model. </t>
+    <t>Statistical measure of polarisation complexity after removal of a thin-screen model.</t>
   </si>
   <si>
     <t>flag_p1</t>
@@ -438,7 +449,7 @@
     <t>meta.code</t>
   </si>
   <si>
-    <t>True if pol_peak_fit is above a threshold value otherwise pol_peak_fit is an upper limit. </t>
+    <t>True if pol_peak_fit is above a threshold value otherwise pol_peak_fit is an upper limit.</t>
   </si>
   <si>
     <t>BOOLEAN</t>
@@ -598,7 +609,7 @@
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="25">
+  <cellXfs count="21">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -609,10 +620,6 @@
     </xf>
     <xf numFmtId="164" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
       <alignment horizontal="center" vertical="top" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="164" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
@@ -668,19 +675,11 @@
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="164" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="164" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="164" fontId="4" fillId="0" borderId="1" xfId="20" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
@@ -689,10 +688,6 @@
     </xf>
     <xf numFmtId="164" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
       <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="left" vertical="top" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="164" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
@@ -707,7 +702,7 @@
     <cellStyle name="Currency" xfId="17" builtinId="4" customBuiltin="false"/>
     <cellStyle name="Currency [0]" xfId="18" builtinId="7" customBuiltin="false"/>
     <cellStyle name="Percent" xfId="19" builtinId="5" customBuiltin="false"/>
-    <cellStyle name="Excel Built-in Neutral" xfId="20" builtinId="54" customBuiltin="true"/>
+    <cellStyle name="Excel Built-in Excel Built-in Neutral" xfId="20" builtinId="54" customBuiltin="true"/>
   </cellStyles>
   <dxfs count="3">
     <dxf>
@@ -821,10 +816,10 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="1:44"/>
+  <dimension ref="1:45"/>
   <sheetViews>
     <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="D3" activeCellId="0" sqref="D3"/>
+      <selection pane="topLeft" activeCell="A4" activeCellId="0" sqref="A4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.95"/>
@@ -835,25 +830,24 @@
     <col collapsed="false" hidden="false" max="4" min="4" style="2" width="12.7125506072875"/>
     <col collapsed="false" hidden="false" max="5" min="5" style="2" width="20.4251012145749"/>
     <col collapsed="false" hidden="false" max="6" min="6" style="3" width="14.8542510121458"/>
-    <col collapsed="false" hidden="false" max="8" min="7" style="4" width="8.85425101214575"/>
-    <col collapsed="false" hidden="false" max="9" min="9" style="3" width="8.85425101214575"/>
+    <col collapsed="false" hidden="false" max="9" min="7" style="3" width="8.85425101214575"/>
     <col collapsed="false" hidden="false" max="10" min="10" style="2" width="60.1417004048583"/>
     <col collapsed="false" hidden="false" max="1025" min="11" style="3" width="8.85425101214575"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="42" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A1" s="5" t="s">
-        <v>0</v>
-      </c>
-      <c r="B1" s="5"/>
-      <c r="C1" s="5"/>
-      <c r="D1" s="5"/>
-      <c r="E1" s="5"/>
+      <c r="A1" s="4" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="4"/>
+      <c r="C1" s="4"/>
+      <c r="D1" s="4"/>
+      <c r="E1" s="4"/>
       <c r="F1" s="0"/>
       <c r="G1" s="0"/>
       <c r="H1" s="0"/>
       <c r="I1" s="0"/>
-      <c r="J1" s="6"/>
+      <c r="J1" s="5"/>
       <c r="K1" s="0"/>
       <c r="L1" s="0"/>
       <c r="M1" s="0"/>
@@ -1869,1276 +1863,1304 @@
       <c r="AMI1" s="0"/>
       <c r="AMJ1" s="0"/>
     </row>
-    <row r="2" s="12" customFormat="true" ht="15.95" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A2" s="7" t="s">
-        <v>1</v>
-      </c>
-      <c r="B2" s="8" t="s">
+    <row r="2" s="11" customFormat="true" ht="15.95" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A2" s="6" t="s">
+        <v>1</v>
+      </c>
+      <c r="B2" s="7" t="s">
         <v>2</v>
       </c>
-      <c r="C2" s="9" t="s">
+      <c r="C2" s="8" t="s">
         <v>3</v>
       </c>
-      <c r="D2" s="9" t="s">
+      <c r="D2" s="8" t="s">
         <v>4</v>
       </c>
-      <c r="E2" s="9" t="s">
+      <c r="E2" s="8" t="s">
         <v>5</v>
       </c>
-      <c r="F2" s="10" t="s">
+      <c r="F2" s="9" t="s">
         <v>6</v>
       </c>
-      <c r="G2" s="9" t="s">
+      <c r="G2" s="8" t="s">
         <v>7</v>
       </c>
-      <c r="H2" s="10" t="s">
+      <c r="H2" s="9" t="s">
         <v>8</v>
       </c>
-      <c r="I2" s="10" t="s">
+      <c r="I2" s="9" t="s">
         <v>9</v>
       </c>
-      <c r="J2" s="9" t="s">
+      <c r="J2" s="8" t="s">
         <v>10</v>
       </c>
-      <c r="K2" s="11"/>
-    </row>
-    <row r="3" s="19" customFormat="true" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A3" s="13" t="s">
+      <c r="K2" s="10"/>
+    </row>
+    <row r="3" s="17" customFormat="true" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A3" s="12" t="s">
         <v>11</v>
       </c>
-      <c r="B3" s="14"/>
-      <c r="C3" s="15" t="s">
+      <c r="B3" s="13"/>
+      <c r="C3" s="14" t="s">
         <v>12</v>
       </c>
-      <c r="D3" s="16" t="s">
+      <c r="D3" s="15" t="s">
         <v>13</v>
       </c>
-      <c r="E3" s="16"/>
-      <c r="F3" s="17" t="n">
-        <v>0</v>
-      </c>
-      <c r="G3" s="17" t="n">
-        <v>0</v>
-      </c>
-      <c r="H3" s="17" t="n">
-        <v>1</v>
-      </c>
-      <c r="I3" s="13" t="n">
-        <v>0</v>
-      </c>
-      <c r="J3" s="18" t="s">
+      <c r="E3" s="15"/>
+      <c r="F3" s="12" t="n">
+        <v>0</v>
+      </c>
+      <c r="G3" s="12" t="n">
+        <v>0</v>
+      </c>
+      <c r="H3" s="12" t="n">
+        <v>1</v>
+      </c>
+      <c r="I3" s="12" t="n">
+        <v>0</v>
+      </c>
+      <c r="J3" s="16" t="s">
         <v>14</v>
       </c>
     </row>
-    <row r="4" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A4" s="13" t="s">
+    <row r="4" s="17" customFormat="true" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A4" s="12" t="s">
         <v>15</v>
       </c>
-      <c r="B4" s="20" t="s">
+      <c r="B4" s="13" t="s">
         <v>16</v>
       </c>
-      <c r="C4" s="20" t="s">
+      <c r="C4" s="14" t="s">
         <v>17</v>
       </c>
-      <c r="D4" s="18" t="s">
+      <c r="D4" s="15" t="s">
         <v>18</v>
       </c>
-      <c r="E4" s="18" t="s">
+      <c r="E4" s="15"/>
+      <c r="F4" s="12" t="n">
+        <v>1</v>
+      </c>
+      <c r="G4" s="12" t="n">
+        <v>0</v>
+      </c>
+      <c r="H4" s="12" t="n">
+        <v>0</v>
+      </c>
+      <c r="I4" s="12" t="n">
+        <v>0</v>
+      </c>
+      <c r="J4" s="16"/>
+    </row>
+    <row r="5" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A5" s="12" t="s">
         <v>19</v>
       </c>
-      <c r="F4" s="17" t="n">
-        <v>0</v>
-      </c>
-      <c r="G4" s="17" t="n">
-        <v>0</v>
-      </c>
-      <c r="H4" s="17" t="n">
-        <v>0</v>
-      </c>
-      <c r="I4" s="13" t="n">
-        <v>0</v>
-      </c>
-      <c r="J4" s="18" t="s">
+      <c r="B5" s="13" t="s">
+        <v>20</v>
+      </c>
+      <c r="C5" s="13" t="s">
+        <v>21</v>
+      </c>
+      <c r="D5" s="16" t="s">
+        <v>22</v>
+      </c>
+      <c r="E5" s="16" t="s">
+        <v>23</v>
+      </c>
+      <c r="F5" s="12" t="n">
+        <v>0</v>
+      </c>
+      <c r="G5" s="12" t="n">
+        <v>0</v>
+      </c>
+      <c r="H5" s="12" t="n">
+        <v>0</v>
+      </c>
+      <c r="I5" s="12" t="n">
+        <v>0</v>
+      </c>
+      <c r="J5" s="16" t="s">
         <v>14</v>
       </c>
     </row>
-    <row r="5" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A5" s="13" t="s">
-        <v>20</v>
-      </c>
-      <c r="B5" s="20" t="s">
-        <v>21</v>
-      </c>
-      <c r="C5" s="20" t="s">
-        <v>22</v>
-      </c>
-      <c r="D5" s="18" t="s">
-        <v>18</v>
-      </c>
-      <c r="E5" s="18" t="s">
-        <v>19</v>
-      </c>
-      <c r="F5" s="17" t="n">
-        <v>0</v>
-      </c>
-      <c r="G5" s="17" t="n">
-        <v>0</v>
-      </c>
-      <c r="H5" s="17" t="n">
-        <v>0</v>
-      </c>
-      <c r="I5" s="13" t="n">
-        <v>0</v>
-      </c>
-      <c r="J5" s="18" t="s">
+    <row r="6" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A6" s="12" t="s">
+        <v>24</v>
+      </c>
+      <c r="B6" s="13" t="s">
+        <v>25</v>
+      </c>
+      <c r="C6" s="13" t="s">
+        <v>26</v>
+      </c>
+      <c r="D6" s="16" t="s">
+        <v>22</v>
+      </c>
+      <c r="E6" s="16" t="s">
+        <v>23</v>
+      </c>
+      <c r="F6" s="12" t="n">
+        <v>0</v>
+      </c>
+      <c r="G6" s="12" t="n">
+        <v>0</v>
+      </c>
+      <c r="H6" s="12" t="n">
+        <v>0</v>
+      </c>
+      <c r="I6" s="12" t="n">
+        <v>0</v>
+      </c>
+      <c r="J6" s="16" t="s">
         <v>14</v>
       </c>
     </row>
-    <row r="6" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A6" s="15" t="s">
+    <row r="7" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A7" s="14" t="s">
+        <v>27</v>
+      </c>
+      <c r="B7" s="18" t="s">
+        <v>28</v>
+      </c>
+      <c r="C7" s="14" t="s">
+        <v>29</v>
+      </c>
+      <c r="D7" s="15" t="s">
+        <v>22</v>
+      </c>
+      <c r="E7" s="15" t="s">
+        <v>30</v>
+      </c>
+      <c r="F7" s="12" t="n">
+        <v>1</v>
+      </c>
+      <c r="G7" s="12" t="n">
+        <v>0</v>
+      </c>
+      <c r="H7" s="12" t="n">
+        <v>0</v>
+      </c>
+      <c r="I7" s="12" t="n">
+        <v>0</v>
+      </c>
+      <c r="J7" s="15"/>
+    </row>
+    <row r="8" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A8" s="14" t="s">
+        <v>31</v>
+      </c>
+      <c r="B8" s="13" t="s">
+        <v>32</v>
+      </c>
+      <c r="C8" s="14" t="s">
+        <v>33</v>
+      </c>
+      <c r="D8" s="15" t="s">
+        <v>22</v>
+      </c>
+      <c r="E8" s="15" t="s">
+        <v>30</v>
+      </c>
+      <c r="F8" s="12" t="n">
+        <v>1</v>
+      </c>
+      <c r="G8" s="12" t="n">
+        <v>0</v>
+      </c>
+      <c r="H8" s="12" t="n">
+        <v>0</v>
+      </c>
+      <c r="I8" s="12" t="n">
+        <v>0</v>
+      </c>
+      <c r="J8" s="15"/>
+    </row>
+    <row r="9" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A9" s="14" t="s">
+        <v>34</v>
+      </c>
+      <c r="B9" s="13" t="s">
+        <v>35</v>
+      </c>
+      <c r="C9" s="14" t="s">
+        <v>36</v>
+      </c>
+      <c r="D9" s="15" t="s">
+        <v>22</v>
+      </c>
+      <c r="E9" s="15" t="s">
+        <v>30</v>
+      </c>
+      <c r="F9" s="12" t="n">
+        <v>1</v>
+      </c>
+      <c r="G9" s="12" t="n">
+        <v>0</v>
+      </c>
+      <c r="H9" s="12" t="n">
+        <v>0</v>
+      </c>
+      <c r="I9" s="12" t="n">
+        <v>0</v>
+      </c>
+      <c r="J9" s="15"/>
+    </row>
+    <row r="10" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A10" s="14" t="s">
+        <v>37</v>
+      </c>
+      <c r="B10" s="13" t="s">
+        <v>38</v>
+      </c>
+      <c r="C10" s="14" t="s">
+        <v>39</v>
+      </c>
+      <c r="D10" s="15" t="s">
+        <v>22</v>
+      </c>
+      <c r="E10" s="15" t="s">
+        <v>30</v>
+      </c>
+      <c r="F10" s="12" t="n">
+        <v>1</v>
+      </c>
+      <c r="G10" s="12" t="n">
+        <v>0</v>
+      </c>
+      <c r="H10" s="12" t="n">
+        <v>0</v>
+      </c>
+      <c r="I10" s="12" t="n">
+        <v>0</v>
+      </c>
+      <c r="J10" s="15"/>
+    </row>
+    <row r="11" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A11" s="14" t="s">
+        <v>40</v>
+      </c>
+      <c r="B11" s="13" t="s">
+        <v>41</v>
+      </c>
+      <c r="C11" s="14" t="s">
+        <v>42</v>
+      </c>
+      <c r="D11" s="15" t="s">
+        <v>22</v>
+      </c>
+      <c r="E11" s="15" t="s">
+        <v>30</v>
+      </c>
+      <c r="F11" s="12" t="n">
+        <v>1</v>
+      </c>
+      <c r="G11" s="12" t="n">
+        <v>0</v>
+      </c>
+      <c r="H11" s="12" t="n">
+        <v>0</v>
+      </c>
+      <c r="I11" s="12" t="n">
+        <v>0</v>
+      </c>
+      <c r="J11" s="15"/>
+    </row>
+    <row r="12" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A12" s="14" t="s">
+        <v>43</v>
+      </c>
+      <c r="B12" s="13" t="s">
+        <v>44</v>
+      </c>
+      <c r="C12" s="14" t="s">
+        <v>45</v>
+      </c>
+      <c r="D12" s="15" t="s">
+        <v>22</v>
+      </c>
+      <c r="E12" s="15" t="s">
+        <v>30</v>
+      </c>
+      <c r="F12" s="12" t="n">
+        <v>1</v>
+      </c>
+      <c r="G12" s="12" t="n">
+        <v>0</v>
+      </c>
+      <c r="H12" s="12" t="n">
+        <v>0</v>
+      </c>
+      <c r="I12" s="12" t="n">
+        <v>0</v>
+      </c>
+      <c r="J12" s="15"/>
+    </row>
+    <row r="13" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A13" s="14" t="s">
+        <v>46</v>
+      </c>
+      <c r="B13" s="13" t="s">
+        <v>47</v>
+      </c>
+      <c r="C13" s="14" t="s">
+        <v>48</v>
+      </c>
+      <c r="D13" s="15" t="s">
+        <v>22</v>
+      </c>
+      <c r="E13" s="15" t="s">
+        <v>30</v>
+      </c>
+      <c r="F13" s="12" t="n">
+        <v>1</v>
+      </c>
+      <c r="G13" s="12" t="n">
+        <v>0</v>
+      </c>
+      <c r="H13" s="12" t="n">
+        <v>0</v>
+      </c>
+      <c r="I13" s="12" t="n">
+        <v>0</v>
+      </c>
+      <c r="J13" s="15"/>
+    </row>
+    <row r="14" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A14" s="14" t="s">
+        <v>49</v>
+      </c>
+      <c r="B14" s="13" t="s">
+        <v>50</v>
+      </c>
+      <c r="C14" s="14" t="s">
+        <v>51</v>
+      </c>
+      <c r="D14" s="15" t="s">
+        <v>22</v>
+      </c>
+      <c r="E14" s="15" t="s">
+        <v>30</v>
+      </c>
+      <c r="F14" s="12" t="n">
+        <v>1</v>
+      </c>
+      <c r="G14" s="12" t="n">
+        <v>0</v>
+      </c>
+      <c r="H14" s="12" t="n">
+        <v>0</v>
+      </c>
+      <c r="I14" s="12" t="n">
+        <v>0</v>
+      </c>
+      <c r="J14" s="15"/>
+    </row>
+    <row r="15" customFormat="false" ht="30" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A15" s="14" t="s">
+        <v>52</v>
+      </c>
+      <c r="B15" s="14" t="s">
+        <v>53</v>
+      </c>
+      <c r="C15" s="14" t="s">
+        <v>54</v>
+      </c>
+      <c r="D15" s="15" t="s">
+        <v>22</v>
+      </c>
+      <c r="E15" s="15"/>
+      <c r="F15" s="12" t="n">
+        <v>1</v>
+      </c>
+      <c r="G15" s="12" t="n">
+        <v>0</v>
+      </c>
+      <c r="H15" s="12" t="n">
+        <v>0</v>
+      </c>
+      <c r="I15" s="12" t="n">
+        <v>0</v>
+      </c>
+      <c r="J15" s="15"/>
+    </row>
+    <row r="16" customFormat="false" ht="30" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A16" s="14" t="s">
+        <v>55</v>
+      </c>
+      <c r="B16" s="14" t="s">
+        <v>53</v>
+      </c>
+      <c r="C16" s="14" t="s">
+        <v>56</v>
+      </c>
+      <c r="D16" s="15" t="s">
+        <v>22</v>
+      </c>
+      <c r="E16" s="15"/>
+      <c r="F16" s="12" t="n">
+        <v>1</v>
+      </c>
+      <c r="G16" s="12" t="n">
+        <v>0</v>
+      </c>
+      <c r="H16" s="12" t="n">
+        <v>0</v>
+      </c>
+      <c r="I16" s="12" t="n">
+        <v>0</v>
+      </c>
+      <c r="J16" s="15"/>
+    </row>
+    <row r="17" customFormat="false" ht="30" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A17" s="14" t="s">
+        <v>57</v>
+      </c>
+      <c r="B17" s="14" t="s">
+        <v>53</v>
+      </c>
+      <c r="C17" s="14" t="s">
+        <v>58</v>
+      </c>
+      <c r="D17" s="15" t="s">
+        <v>22</v>
+      </c>
+      <c r="E17" s="15"/>
+      <c r="F17" s="12" t="n">
+        <v>1</v>
+      </c>
+      <c r="G17" s="12" t="n">
+        <v>0</v>
+      </c>
+      <c r="H17" s="12" t="n">
+        <v>0</v>
+      </c>
+      <c r="I17" s="12" t="n">
+        <v>0</v>
+      </c>
+      <c r="J17" s="15"/>
+    </row>
+    <row r="18" customFormat="false" ht="30" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A18" s="14" t="s">
+        <v>59</v>
+      </c>
+      <c r="B18" s="14" t="s">
+        <v>53</v>
+      </c>
+      <c r="C18" s="14" t="s">
+        <v>60</v>
+      </c>
+      <c r="D18" s="15" t="s">
+        <v>22</v>
+      </c>
+      <c r="E18" s="15"/>
+      <c r="F18" s="12" t="n">
+        <v>1</v>
+      </c>
+      <c r="G18" s="12" t="n">
+        <v>0</v>
+      </c>
+      <c r="H18" s="12" t="n">
+        <v>0</v>
+      </c>
+      <c r="I18" s="12" t="n">
+        <v>0</v>
+      </c>
+      <c r="J18" s="15"/>
+    </row>
+    <row r="19" customFormat="false" ht="30" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A19" s="14" t="s">
+        <v>61</v>
+      </c>
+      <c r="B19" s="14" t="s">
+        <v>53</v>
+      </c>
+      <c r="C19" s="14" t="s">
+        <v>62</v>
+      </c>
+      <c r="D19" s="15" t="s">
+        <v>22</v>
+      </c>
+      <c r="E19" s="15"/>
+      <c r="F19" s="12" t="n">
+        <v>1</v>
+      </c>
+      <c r="G19" s="12" t="n">
+        <v>0</v>
+      </c>
+      <c r="H19" s="12" t="n">
+        <v>0</v>
+      </c>
+      <c r="I19" s="12" t="n">
+        <v>0</v>
+      </c>
+      <c r="J19" s="15"/>
+    </row>
+    <row r="20" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A20" s="14" t="s">
+        <v>63</v>
+      </c>
+      <c r="B20" s="14" t="s">
+        <v>64</v>
+      </c>
+      <c r="C20" s="14" t="s">
+        <v>65</v>
+      </c>
+      <c r="D20" s="15" t="s">
+        <v>22</v>
+      </c>
+      <c r="E20" s="15" t="s">
+        <v>66</v>
+      </c>
+      <c r="F20" s="12" t="n">
+        <v>1</v>
+      </c>
+      <c r="G20" s="12" t="n">
+        <v>0</v>
+      </c>
+      <c r="H20" s="12" t="n">
+        <v>0</v>
+      </c>
+      <c r="I20" s="12" t="n">
+        <v>1</v>
+      </c>
+      <c r="J20" s="15"/>
+    </row>
+    <row r="21" customFormat="false" ht="30" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A21" s="14" t="s">
+        <v>67</v>
+      </c>
+      <c r="B21" s="19" t="s">
+        <v>68</v>
+      </c>
+      <c r="C21" s="14" t="s">
+        <v>69</v>
+      </c>
+      <c r="D21" s="15" t="s">
+        <v>22</v>
+      </c>
+      <c r="E21" s="15" t="s">
+        <v>70</v>
+      </c>
+      <c r="F21" s="12" t="n">
+        <v>1</v>
+      </c>
+      <c r="G21" s="12" t="n">
+        <v>0</v>
+      </c>
+      <c r="H21" s="12" t="n">
+        <v>0</v>
+      </c>
+      <c r="I21" s="12" t="n">
+        <v>0</v>
+      </c>
+      <c r="J21" s="15"/>
+    </row>
+    <row r="22" customFormat="false" ht="30" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A22" s="14" t="s">
+        <v>71</v>
+      </c>
+      <c r="B22" s="14" t="s">
+        <v>72</v>
+      </c>
+      <c r="C22" s="14" t="s">
+        <v>73</v>
+      </c>
+      <c r="D22" s="15" t="s">
+        <v>22</v>
+      </c>
+      <c r="E22" s="15" t="s">
+        <v>30</v>
+      </c>
+      <c r="F22" s="12" t="n">
+        <v>1</v>
+      </c>
+      <c r="G22" s="12" t="n">
+        <v>0</v>
+      </c>
+      <c r="H22" s="12" t="n">
+        <v>0</v>
+      </c>
+      <c r="I22" s="12" t="n">
+        <v>0</v>
+      </c>
+      <c r="J22" s="15"/>
+    </row>
+    <row r="23" customFormat="false" ht="30" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A23" s="14" t="s">
+        <v>74</v>
+      </c>
+      <c r="B23" s="14" t="s">
+        <v>75</v>
+      </c>
+      <c r="C23" s="14" t="s">
+        <v>76</v>
+      </c>
+      <c r="D23" s="15" t="s">
+        <v>22</v>
+      </c>
+      <c r="E23" s="15" t="s">
+        <v>30</v>
+      </c>
+      <c r="F23" s="12" t="n">
+        <v>1</v>
+      </c>
+      <c r="G23" s="12" t="n">
+        <v>0</v>
+      </c>
+      <c r="H23" s="12" t="n">
+        <v>0</v>
+      </c>
+      <c r="I23" s="12" t="n">
+        <v>0</v>
+      </c>
+      <c r="J23" s="15"/>
+    </row>
+    <row r="24" customFormat="false" ht="30" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A24" s="14" t="s">
+        <v>77</v>
+      </c>
+      <c r="B24" s="14" t="s">
+        <v>78</v>
+      </c>
+      <c r="C24" s="14" t="s">
+        <v>79</v>
+      </c>
+      <c r="D24" s="15" t="s">
+        <v>22</v>
+      </c>
+      <c r="E24" s="15" t="s">
+        <v>30</v>
+      </c>
+      <c r="F24" s="12" t="n">
+        <v>1</v>
+      </c>
+      <c r="G24" s="12" t="n">
+        <v>0</v>
+      </c>
+      <c r="H24" s="12" t="n">
+        <v>0</v>
+      </c>
+      <c r="I24" s="12" t="n">
+        <v>0</v>
+      </c>
+      <c r="J24" s="15"/>
+    </row>
+    <row r="25" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A25" s="14" t="s">
+        <v>80</v>
+      </c>
+      <c r="B25" s="14" t="s">
+        <v>81</v>
+      </c>
+      <c r="C25" s="14" t="s">
+        <v>82</v>
+      </c>
+      <c r="D25" s="15" t="s">
+        <v>22</v>
+      </c>
+      <c r="E25" s="15" t="s">
+        <v>30</v>
+      </c>
+      <c r="F25" s="12" t="n">
+        <v>1</v>
+      </c>
+      <c r="G25" s="12" t="n">
+        <v>0</v>
+      </c>
+      <c r="H25" s="12" t="n">
+        <v>0</v>
+      </c>
+      <c r="I25" s="12" t="n">
+        <v>1</v>
+      </c>
+      <c r="J25" s="15"/>
+    </row>
+    <row r="26" customFormat="false" ht="30" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A26" s="14" t="s">
+        <v>83</v>
+      </c>
+      <c r="B26" s="14" t="s">
+        <v>84</v>
+      </c>
+      <c r="C26" s="14" t="s">
+        <v>85</v>
+      </c>
+      <c r="D26" s="15" t="s">
+        <v>22</v>
+      </c>
+      <c r="E26" s="15" t="s">
+        <v>30</v>
+      </c>
+      <c r="F26" s="12" t="n">
+        <v>1</v>
+      </c>
+      <c r="G26" s="12" t="n">
+        <v>0</v>
+      </c>
+      <c r="H26" s="12" t="n">
+        <v>0</v>
+      </c>
+      <c r="I26" s="12" t="n">
+        <v>1</v>
+      </c>
+      <c r="J26" s="15"/>
+    </row>
+    <row r="27" customFormat="false" ht="30" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A27" s="14" t="s">
+        <v>86</v>
+      </c>
+      <c r="B27" s="14" t="s">
+        <v>87</v>
+      </c>
+      <c r="C27" s="14" t="s">
+        <v>88</v>
+      </c>
+      <c r="D27" s="15" t="s">
+        <v>22</v>
+      </c>
+      <c r="E27" s="15" t="s">
+        <v>30</v>
+      </c>
+      <c r="F27" s="12" t="n">
+        <v>1</v>
+      </c>
+      <c r="G27" s="12" t="n">
+        <v>0</v>
+      </c>
+      <c r="H27" s="12" t="n">
+        <v>0</v>
+      </c>
+      <c r="I27" s="12" t="n">
+        <v>1</v>
+      </c>
+      <c r="J27" s="15"/>
+    </row>
+    <row r="28" customFormat="false" ht="30" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A28" s="14" t="s">
+        <v>89</v>
+      </c>
+      <c r="B28" s="14" t="s">
+        <v>90</v>
+      </c>
+      <c r="C28" s="14" t="s">
+        <v>91</v>
+      </c>
+      <c r="D28" s="15" t="s">
+        <v>22</v>
+      </c>
+      <c r="E28" s="15"/>
+      <c r="F28" s="12" t="n">
+        <v>1</v>
+      </c>
+      <c r="G28" s="12" t="n">
+        <v>0</v>
+      </c>
+      <c r="H28" s="12" t="n">
+        <v>0</v>
+      </c>
+      <c r="I28" s="12" t="n">
+        <v>1</v>
+      </c>
+      <c r="J28" s="15"/>
+    </row>
+    <row r="29" customFormat="false" ht="30" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A29" s="14" t="s">
+        <v>92</v>
+      </c>
+      <c r="B29" s="14" t="s">
+        <v>93</v>
+      </c>
+      <c r="C29" s="14" t="s">
+        <v>94</v>
+      </c>
+      <c r="D29" s="15" t="s">
+        <v>22</v>
+      </c>
+      <c r="E29" s="15"/>
+      <c r="F29" s="12" t="n">
+        <v>1</v>
+      </c>
+      <c r="G29" s="12" t="n">
+        <v>0</v>
+      </c>
+      <c r="H29" s="12" t="n">
+        <v>0</v>
+      </c>
+      <c r="I29" s="12" t="n">
+        <v>1</v>
+      </c>
+      <c r="J29" s="15"/>
+    </row>
+    <row r="30" customFormat="false" ht="30" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A30" s="14" t="s">
+        <v>95</v>
+      </c>
+      <c r="B30" s="13" t="s">
+        <v>96</v>
+      </c>
+      <c r="C30" s="14" t="s">
+        <v>97</v>
+      </c>
+      <c r="D30" s="15" t="s">
+        <v>22</v>
+      </c>
+      <c r="E30" s="15" t="s">
+        <v>70</v>
+      </c>
+      <c r="F30" s="12" t="n">
+        <v>1</v>
+      </c>
+      <c r="G30" s="12" t="n">
+        <v>0</v>
+      </c>
+      <c r="H30" s="12" t="n">
+        <v>0</v>
+      </c>
+      <c r="I30" s="12" t="n">
+        <v>0</v>
+      </c>
+      <c r="J30" s="15"/>
+    </row>
+    <row r="31" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A31" s="14" t="s">
+        <v>98</v>
+      </c>
+      <c r="B31" s="13" t="s">
+        <v>99</v>
+      </c>
+      <c r="C31" s="14" t="s">
+        <v>100</v>
+      </c>
+      <c r="D31" s="15" t="s">
+        <v>22</v>
+      </c>
+      <c r="E31" s="15" t="s">
+        <v>70</v>
+      </c>
+      <c r="F31" s="12" t="n">
+        <v>1</v>
+      </c>
+      <c r="G31" s="12" t="n">
+        <v>0</v>
+      </c>
+      <c r="H31" s="12" t="n">
+        <v>0</v>
+      </c>
+      <c r="I31" s="12" t="n">
+        <v>0</v>
+      </c>
+      <c r="J31" s="15"/>
+    </row>
+    <row r="32" customFormat="false" ht="30" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A32" s="20" t="s">
+        <v>101</v>
+      </c>
+      <c r="B32" s="13" t="s">
+        <v>102</v>
+      </c>
+      <c r="C32" s="20" t="s">
+        <v>103</v>
+      </c>
+      <c r="D32" s="15" t="s">
+        <v>22</v>
+      </c>
+      <c r="E32" s="15" t="s">
+        <v>70</v>
+      </c>
+      <c r="F32" s="12" t="n">
+        <v>1</v>
+      </c>
+      <c r="G32" s="12" t="n">
+        <v>0</v>
+      </c>
+      <c r="H32" s="12" t="n">
+        <v>0</v>
+      </c>
+      <c r="I32" s="12" t="n">
+        <v>1</v>
+      </c>
+      <c r="J32" s="15"/>
+    </row>
+    <row r="33" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A33" s="20" t="s">
+        <v>104</v>
+      </c>
+      <c r="B33" s="13" t="s">
+        <v>105</v>
+      </c>
+      <c r="C33" s="20" t="s">
+        <v>106</v>
+      </c>
+      <c r="D33" s="15" t="s">
+        <v>22</v>
+      </c>
+      <c r="E33" s="15" t="s">
+        <v>70</v>
+      </c>
+      <c r="F33" s="12" t="n">
+        <v>1</v>
+      </c>
+      <c r="G33" s="12" t="n">
+        <v>0</v>
+      </c>
+      <c r="H33" s="12" t="n">
+        <v>0</v>
+      </c>
+      <c r="I33" s="12" t="n">
+        <v>1</v>
+      </c>
+      <c r="J33" s="15"/>
+    </row>
+    <row r="34" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A34" s="14" t="s">
+        <v>107</v>
+      </c>
+      <c r="B34" s="14" t="s">
+        <v>108</v>
+      </c>
+      <c r="C34" s="14" t="s">
+        <v>109</v>
+      </c>
+      <c r="D34" s="15" t="s">
+        <v>22</v>
+      </c>
+      <c r="E34" s="15" t="s">
         <v>23</v>
       </c>
-      <c r="B6" s="21" t="s">
-        <v>24</v>
-      </c>
-      <c r="C6" s="15" t="s">
-        <v>25</v>
-      </c>
-      <c r="D6" s="16" t="s">
-        <v>18</v>
-      </c>
-      <c r="E6" s="16" t="s">
-        <v>26</v>
-      </c>
-      <c r="F6" s="17" t="n">
-        <v>1</v>
-      </c>
-      <c r="G6" s="17" t="n">
-        <v>0</v>
-      </c>
-      <c r="H6" s="17" t="n">
-        <v>0</v>
-      </c>
-      <c r="I6" s="13" t="n">
-        <v>0</v>
-      </c>
-      <c r="J6" s="16"/>
-    </row>
-    <row r="7" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A7" s="15" t="s">
-        <v>27</v>
-      </c>
-      <c r="B7" s="14" t="s">
-        <v>28</v>
-      </c>
-      <c r="C7" s="15" t="s">
-        <v>29</v>
-      </c>
-      <c r="D7" s="16" t="s">
-        <v>18</v>
-      </c>
-      <c r="E7" s="16" t="s">
-        <v>26</v>
-      </c>
-      <c r="F7" s="17" t="n">
-        <v>1</v>
-      </c>
-      <c r="G7" s="17" t="n">
-        <v>0</v>
-      </c>
-      <c r="H7" s="17" t="n">
-        <v>0</v>
-      </c>
-      <c r="I7" s="13" t="n">
-        <v>0</v>
-      </c>
-      <c r="J7" s="16"/>
-    </row>
-    <row r="8" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A8" s="15" t="s">
-        <v>30</v>
-      </c>
-      <c r="B8" s="14" t="s">
-        <v>31</v>
-      </c>
-      <c r="C8" s="15" t="s">
-        <v>32</v>
-      </c>
-      <c r="D8" s="16" t="s">
-        <v>18</v>
-      </c>
-      <c r="E8" s="16" t="s">
-        <v>26</v>
-      </c>
-      <c r="F8" s="17" t="n">
-        <v>1</v>
-      </c>
-      <c r="G8" s="17" t="n">
-        <v>0</v>
-      </c>
-      <c r="H8" s="17" t="n">
-        <v>0</v>
-      </c>
-      <c r="I8" s="13" t="n">
-        <v>0</v>
-      </c>
-      <c r="J8" s="16"/>
-    </row>
-    <row r="9" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A9" s="15" t="s">
-        <v>33</v>
-      </c>
-      <c r="B9" s="14" t="s">
-        <v>34</v>
-      </c>
-      <c r="C9" s="15" t="s">
-        <v>35</v>
-      </c>
-      <c r="D9" s="16" t="s">
-        <v>18</v>
-      </c>
-      <c r="E9" s="16" t="s">
-        <v>26</v>
-      </c>
-      <c r="F9" s="17" t="n">
-        <v>1</v>
-      </c>
-      <c r="G9" s="17" t="n">
-        <v>0</v>
-      </c>
-      <c r="H9" s="17" t="n">
-        <v>0</v>
-      </c>
-      <c r="I9" s="13" t="n">
-        <v>0</v>
-      </c>
-      <c r="J9" s="16"/>
-    </row>
-    <row r="10" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A10" s="15" t="s">
-        <v>36</v>
-      </c>
-      <c r="B10" s="20" t="s">
-        <v>37</v>
-      </c>
-      <c r="C10" s="15" t="s">
-        <v>38</v>
-      </c>
-      <c r="D10" s="16" t="s">
-        <v>18</v>
-      </c>
-      <c r="E10" s="16" t="s">
-        <v>26</v>
-      </c>
-      <c r="F10" s="17" t="n">
-        <v>1</v>
-      </c>
-      <c r="G10" s="17" t="n">
-        <v>0</v>
-      </c>
-      <c r="H10" s="17" t="n">
-        <v>0</v>
-      </c>
-      <c r="I10" s="13" t="n">
-        <v>0</v>
-      </c>
-      <c r="J10" s="16"/>
-    </row>
-    <row r="11" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A11" s="15" t="s">
-        <v>39</v>
-      </c>
-      <c r="B11" s="14" t="s">
-        <v>40</v>
-      </c>
-      <c r="C11" s="15" t="s">
-        <v>41</v>
-      </c>
-      <c r="D11" s="16" t="s">
-        <v>18</v>
-      </c>
-      <c r="E11" s="16" t="s">
-        <v>26</v>
-      </c>
-      <c r="F11" s="17" t="n">
-        <v>1</v>
-      </c>
-      <c r="G11" s="17" t="n">
-        <v>0</v>
-      </c>
-      <c r="H11" s="17" t="n">
-        <v>0</v>
-      </c>
-      <c r="I11" s="13" t="n">
-        <v>0</v>
-      </c>
-      <c r="J11" s="16"/>
-    </row>
-    <row r="12" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A12" s="15" t="s">
-        <v>42</v>
-      </c>
-      <c r="B12" s="14" t="s">
-        <v>43</v>
-      </c>
-      <c r="C12" s="15" t="s">
-        <v>44</v>
-      </c>
-      <c r="D12" s="16" t="s">
-        <v>18</v>
-      </c>
-      <c r="E12" s="16" t="s">
-        <v>26</v>
-      </c>
-      <c r="F12" s="17" t="n">
-        <v>1</v>
-      </c>
-      <c r="G12" s="17" t="n">
-        <v>0</v>
-      </c>
-      <c r="H12" s="17" t="n">
-        <v>0</v>
-      </c>
-      <c r="I12" s="13" t="n">
-        <v>0</v>
-      </c>
-      <c r="J12" s="16"/>
-    </row>
-    <row r="13" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A13" s="15" t="s">
-        <v>45</v>
-      </c>
-      <c r="B13" s="14" t="s">
-        <v>46</v>
-      </c>
-      <c r="C13" s="15" t="s">
-        <v>47</v>
-      </c>
-      <c r="D13" s="16" t="s">
-        <v>18</v>
-      </c>
-      <c r="E13" s="16" t="s">
-        <v>26</v>
-      </c>
-      <c r="F13" s="17" t="n">
-        <v>1</v>
-      </c>
-      <c r="G13" s="17" t="n">
-        <v>0</v>
-      </c>
-      <c r="H13" s="17" t="n">
-        <v>0</v>
-      </c>
-      <c r="I13" s="13" t="n">
-        <v>0</v>
-      </c>
-      <c r="J13" s="16"/>
-    </row>
-    <row r="14" customFormat="false" ht="30" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A14" s="15" t="s">
-        <v>48</v>
-      </c>
-      <c r="B14" s="15" t="s">
-        <v>49</v>
-      </c>
-      <c r="C14" s="15" t="s">
-        <v>50</v>
-      </c>
-      <c r="D14" s="16" t="s">
-        <v>18</v>
-      </c>
-      <c r="E14" s="16"/>
-      <c r="F14" s="17" t="n">
-        <v>1</v>
-      </c>
-      <c r="G14" s="17" t="n">
-        <v>0</v>
-      </c>
-      <c r="H14" s="17" t="n">
-        <v>0</v>
-      </c>
-      <c r="I14" s="13" t="n">
-        <v>0</v>
-      </c>
-      <c r="J14" s="16"/>
-    </row>
-    <row r="15" customFormat="false" ht="30" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A15" s="15" t="s">
-        <v>51</v>
-      </c>
-      <c r="B15" s="15" t="s">
-        <v>49</v>
-      </c>
-      <c r="C15" s="15" t="s">
-        <v>52</v>
-      </c>
-      <c r="D15" s="16" t="s">
-        <v>18</v>
-      </c>
-      <c r="E15" s="16"/>
-      <c r="F15" s="17" t="n">
-        <v>1</v>
-      </c>
-      <c r="G15" s="17" t="n">
-        <v>0</v>
-      </c>
-      <c r="H15" s="17" t="n">
-        <v>0</v>
-      </c>
-      <c r="I15" s="13" t="n">
-        <v>0</v>
-      </c>
-      <c r="J15" s="16"/>
-    </row>
-    <row r="16" customFormat="false" ht="30" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A16" s="15" t="s">
-        <v>53</v>
-      </c>
-      <c r="B16" s="15" t="s">
-        <v>49</v>
-      </c>
-      <c r="C16" s="15" t="s">
-        <v>54</v>
-      </c>
-      <c r="D16" s="16" t="s">
-        <v>18</v>
-      </c>
-      <c r="E16" s="16"/>
-      <c r="F16" s="17" t="n">
-        <v>1</v>
-      </c>
-      <c r="G16" s="17" t="n">
-        <v>0</v>
-      </c>
-      <c r="H16" s="17" t="n">
-        <v>0</v>
-      </c>
-      <c r="I16" s="13" t="n">
-        <v>0</v>
-      </c>
-      <c r="J16" s="16"/>
-    </row>
-    <row r="17" customFormat="false" ht="30" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A17" s="15" t="s">
-        <v>55</v>
-      </c>
-      <c r="B17" s="15" t="s">
-        <v>49</v>
-      </c>
-      <c r="C17" s="15" t="s">
-        <v>56</v>
-      </c>
-      <c r="D17" s="16" t="s">
-        <v>18</v>
-      </c>
-      <c r="E17" s="16"/>
-      <c r="F17" s="17" t="n">
-        <v>1</v>
-      </c>
-      <c r="G17" s="17" t="n">
-        <v>0</v>
-      </c>
-      <c r="H17" s="17" t="n">
-        <v>0</v>
-      </c>
-      <c r="I17" s="13" t="n">
-        <v>0</v>
-      </c>
-      <c r="J17" s="16"/>
-    </row>
-    <row r="18" customFormat="false" ht="30" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A18" s="15" t="s">
-        <v>57</v>
-      </c>
-      <c r="B18" s="15" t="s">
-        <v>49</v>
-      </c>
-      <c r="C18" s="15" t="s">
-        <v>58</v>
-      </c>
-      <c r="D18" s="16" t="s">
-        <v>18</v>
-      </c>
-      <c r="E18" s="16"/>
-      <c r="F18" s="17" t="n">
-        <v>1</v>
-      </c>
-      <c r="G18" s="17" t="n">
-        <v>0</v>
-      </c>
-      <c r="H18" s="17" t="n">
-        <v>0</v>
-      </c>
-      <c r="I18" s="13" t="n">
-        <v>0</v>
-      </c>
-      <c r="J18" s="16"/>
-    </row>
-    <row r="19" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A19" s="15" t="s">
-        <v>59</v>
-      </c>
-      <c r="B19" s="15" t="s">
-        <v>60</v>
-      </c>
-      <c r="C19" s="15" t="s">
-        <v>61</v>
-      </c>
-      <c r="D19" s="16" t="s">
-        <v>18</v>
-      </c>
-      <c r="E19" s="16" t="s">
-        <v>62</v>
-      </c>
-      <c r="F19" s="17" t="n">
-        <v>1</v>
-      </c>
-      <c r="G19" s="17" t="n">
-        <v>0</v>
-      </c>
-      <c r="H19" s="17" t="n">
-        <v>0</v>
-      </c>
-      <c r="I19" s="13" t="n">
-        <v>1</v>
-      </c>
-      <c r="J19" s="16"/>
-    </row>
-    <row r="20" customFormat="false" ht="30" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A20" s="15" t="s">
-        <v>63</v>
-      </c>
-      <c r="B20" s="22" t="s">
-        <v>64</v>
-      </c>
-      <c r="C20" s="15" t="s">
-        <v>65</v>
-      </c>
-      <c r="D20" s="16" t="s">
-        <v>18</v>
-      </c>
-      <c r="E20" s="16" t="s">
-        <v>66</v>
-      </c>
-      <c r="F20" s="17" t="n">
-        <v>1</v>
-      </c>
-      <c r="G20" s="17" t="n">
-        <v>0</v>
-      </c>
-      <c r="H20" s="17" t="n">
-        <v>0</v>
-      </c>
-      <c r="I20" s="13" t="n">
-        <v>0</v>
-      </c>
-      <c r="J20" s="16"/>
-    </row>
-    <row r="21" customFormat="false" ht="30" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A21" s="15" t="s">
-        <v>67</v>
-      </c>
-      <c r="B21" s="15" t="s">
-        <v>68</v>
-      </c>
-      <c r="C21" s="15" t="s">
-        <v>69</v>
-      </c>
-      <c r="D21" s="16" t="s">
-        <v>18</v>
-      </c>
-      <c r="E21" s="16" t="s">
-        <v>26</v>
-      </c>
-      <c r="F21" s="17" t="n">
-        <v>1</v>
-      </c>
-      <c r="G21" s="17" t="n">
-        <v>0</v>
-      </c>
-      <c r="H21" s="17" t="n">
-        <v>0</v>
-      </c>
-      <c r="I21" s="13" t="n">
-        <v>0</v>
-      </c>
-      <c r="J21" s="16"/>
-    </row>
-    <row r="22" customFormat="false" ht="30" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A22" s="15" t="s">
-        <v>70</v>
-      </c>
-      <c r="B22" s="15" t="s">
-        <v>71</v>
-      </c>
-      <c r="C22" s="15" t="s">
-        <v>72</v>
-      </c>
-      <c r="D22" s="16" t="s">
-        <v>18</v>
-      </c>
-      <c r="E22" s="16" t="s">
-        <v>26</v>
-      </c>
-      <c r="F22" s="17" t="n">
-        <v>1</v>
-      </c>
-      <c r="G22" s="17" t="n">
-        <v>0</v>
-      </c>
-      <c r="H22" s="17" t="n">
-        <v>0</v>
-      </c>
-      <c r="I22" s="13" t="n">
-        <v>0</v>
-      </c>
-      <c r="J22" s="16"/>
-    </row>
-    <row r="23" customFormat="false" ht="30" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A23" s="15" t="s">
-        <v>73</v>
-      </c>
-      <c r="B23" s="15" t="s">
-        <v>74</v>
-      </c>
-      <c r="C23" s="15" t="s">
-        <v>75</v>
-      </c>
-      <c r="D23" s="16" t="s">
-        <v>18</v>
-      </c>
-      <c r="E23" s="16" t="s">
-        <v>26</v>
-      </c>
-      <c r="F23" s="17" t="n">
-        <v>1</v>
-      </c>
-      <c r="G23" s="17" t="n">
-        <v>0</v>
-      </c>
-      <c r="H23" s="17" t="n">
-        <v>0</v>
-      </c>
-      <c r="I23" s="13" t="n">
-        <v>0</v>
-      </c>
-      <c r="J23" s="16"/>
-    </row>
-    <row r="24" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A24" s="15" t="s">
-        <v>76</v>
-      </c>
-      <c r="B24" s="23" t="s">
-        <v>77</v>
-      </c>
-      <c r="C24" s="15" t="s">
-        <v>78</v>
-      </c>
-      <c r="D24" s="16" t="s">
-        <v>18</v>
-      </c>
-      <c r="E24" s="16" t="s">
-        <v>26</v>
-      </c>
-      <c r="F24" s="17" t="n">
-        <v>1</v>
-      </c>
-      <c r="G24" s="17" t="n">
-        <v>0</v>
-      </c>
-      <c r="H24" s="17" t="n">
-        <v>0</v>
-      </c>
-      <c r="I24" s="13" t="n">
-        <v>1</v>
-      </c>
-      <c r="J24" s="16"/>
-    </row>
-    <row r="25" customFormat="false" ht="30" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A25" s="15" t="s">
-        <v>79</v>
-      </c>
-      <c r="B25" s="23" t="s">
-        <v>80</v>
-      </c>
-      <c r="C25" s="15" t="s">
-        <v>81</v>
-      </c>
-      <c r="D25" s="16" t="s">
-        <v>18</v>
-      </c>
-      <c r="E25" s="16" t="s">
-        <v>26</v>
-      </c>
-      <c r="F25" s="17" t="n">
-        <v>1</v>
-      </c>
-      <c r="G25" s="17" t="n">
-        <v>0</v>
-      </c>
-      <c r="H25" s="17" t="n">
-        <v>0</v>
-      </c>
-      <c r="I25" s="13" t="n">
-        <v>1</v>
-      </c>
-      <c r="J25" s="16"/>
-    </row>
-    <row r="26" customFormat="false" ht="30" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A26" s="15" t="s">
-        <v>82</v>
-      </c>
-      <c r="B26" s="23" t="s">
-        <v>83</v>
-      </c>
-      <c r="C26" s="15" t="s">
-        <v>84</v>
-      </c>
-      <c r="D26" s="16" t="s">
-        <v>18</v>
-      </c>
-      <c r="E26" s="16" t="s">
-        <v>26</v>
-      </c>
-      <c r="F26" s="17" t="n">
-        <v>1</v>
-      </c>
-      <c r="G26" s="17" t="n">
-        <v>0</v>
-      </c>
-      <c r="H26" s="17" t="n">
-        <v>0</v>
-      </c>
-      <c r="I26" s="13" t="n">
-        <v>1</v>
-      </c>
-      <c r="J26" s="16"/>
-    </row>
-    <row r="27" customFormat="false" ht="30" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A27" s="15" t="s">
-        <v>85</v>
-      </c>
-      <c r="B27" s="23" t="s">
-        <v>86</v>
-      </c>
-      <c r="C27" s="15" t="s">
-        <v>87</v>
-      </c>
-      <c r="D27" s="16" t="s">
-        <v>18</v>
-      </c>
-      <c r="E27" s="16"/>
-      <c r="F27" s="17" t="n">
-        <v>1</v>
-      </c>
-      <c r="G27" s="17" t="n">
-        <v>0</v>
-      </c>
-      <c r="H27" s="17" t="n">
-        <v>0</v>
-      </c>
-      <c r="I27" s="13" t="n">
-        <v>1</v>
-      </c>
-      <c r="J27" s="16"/>
-    </row>
-    <row r="28" customFormat="false" ht="30" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A28" s="15" t="s">
-        <v>88</v>
-      </c>
-      <c r="B28" s="23" t="s">
-        <v>89</v>
-      </c>
-      <c r="C28" s="15" t="s">
-        <v>90</v>
-      </c>
-      <c r="D28" s="16" t="s">
-        <v>18</v>
-      </c>
-      <c r="E28" s="16"/>
-      <c r="F28" s="17" t="n">
-        <v>1</v>
-      </c>
-      <c r="G28" s="17" t="n">
-        <v>0</v>
-      </c>
-      <c r="H28" s="17" t="n">
-        <v>0</v>
-      </c>
-      <c r="I28" s="13" t="n">
-        <v>1</v>
-      </c>
-      <c r="J28" s="16"/>
-    </row>
-    <row r="29" customFormat="false" ht="30" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A29" s="15" t="s">
-        <v>91</v>
-      </c>
-      <c r="B29" s="14" t="s">
-        <v>92</v>
-      </c>
-      <c r="C29" s="15" t="s">
-        <v>93</v>
-      </c>
-      <c r="D29" s="16" t="s">
-        <v>18</v>
-      </c>
-      <c r="E29" s="16" t="s">
-        <v>66</v>
-      </c>
-      <c r="F29" s="17" t="n">
-        <v>1</v>
-      </c>
-      <c r="G29" s="17" t="n">
-        <v>0</v>
-      </c>
-      <c r="H29" s="17" t="n">
-        <v>0</v>
-      </c>
-      <c r="I29" s="13" t="n">
-        <v>0</v>
-      </c>
-      <c r="J29" s="16"/>
-    </row>
-    <row r="30" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A30" s="15" t="s">
-        <v>94</v>
-      </c>
-      <c r="B30" s="14" t="s">
-        <v>95</v>
-      </c>
-      <c r="C30" s="15" t="s">
-        <v>96</v>
-      </c>
-      <c r="D30" s="16" t="s">
-        <v>18</v>
-      </c>
-      <c r="E30" s="16" t="s">
-        <v>66</v>
-      </c>
-      <c r="F30" s="17" t="n">
-        <v>1</v>
-      </c>
-      <c r="G30" s="17" t="n">
-        <v>0</v>
-      </c>
-      <c r="H30" s="17" t="n">
-        <v>0</v>
-      </c>
-      <c r="I30" s="13" t="n">
-        <v>0</v>
-      </c>
-      <c r="J30" s="16"/>
-    </row>
-    <row r="31" customFormat="false" ht="30" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A31" s="24" t="s">
-        <v>97</v>
-      </c>
-      <c r="B31" s="14" t="s">
-        <v>98</v>
-      </c>
-      <c r="C31" s="24" t="s">
-        <v>99</v>
-      </c>
-      <c r="D31" s="16" t="s">
-        <v>18</v>
-      </c>
-      <c r="E31" s="16" t="s">
-        <v>66</v>
-      </c>
-      <c r="F31" s="17" t="n">
-        <v>1</v>
-      </c>
-      <c r="G31" s="17" t="n">
-        <v>0</v>
-      </c>
-      <c r="H31" s="17" t="n">
-        <v>0</v>
-      </c>
-      <c r="I31" s="13" t="n">
-        <v>1</v>
-      </c>
-      <c r="J31" s="16"/>
-    </row>
-    <row r="32" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A32" s="24" t="s">
-        <v>100</v>
-      </c>
-      <c r="B32" s="14" t="s">
-        <v>101</v>
-      </c>
-      <c r="C32" s="24" t="s">
-        <v>102</v>
-      </c>
-      <c r="D32" s="16" t="s">
-        <v>18</v>
-      </c>
-      <c r="E32" s="16" t="s">
-        <v>66</v>
-      </c>
-      <c r="F32" s="17" t="n">
-        <v>1</v>
-      </c>
-      <c r="G32" s="17" t="n">
-        <v>0</v>
-      </c>
-      <c r="H32" s="17" t="n">
-        <v>0</v>
-      </c>
-      <c r="I32" s="13" t="n">
-        <v>1</v>
-      </c>
-      <c r="J32" s="16"/>
-    </row>
-    <row r="33" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A33" s="15" t="s">
-        <v>103</v>
-      </c>
-      <c r="B33" s="15" t="s">
-        <v>104</v>
-      </c>
-      <c r="C33" s="15" t="s">
-        <v>105</v>
-      </c>
-      <c r="D33" s="16" t="s">
-        <v>18</v>
-      </c>
-      <c r="E33" s="16" t="s">
-        <v>19</v>
-      </c>
-      <c r="F33" s="17" t="n">
-        <v>1</v>
-      </c>
-      <c r="G33" s="17" t="n">
-        <v>0</v>
-      </c>
-      <c r="H33" s="17" t="n">
-        <v>0</v>
-      </c>
-      <c r="I33" s="13" t="n">
-        <v>0</v>
-      </c>
-      <c r="J33" s="16"/>
-    </row>
-    <row r="34" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A34" s="15" t="s">
-        <v>106</v>
-      </c>
-      <c r="B34" s="15" t="s">
-        <v>107</v>
-      </c>
-      <c r="C34" s="15" t="s">
-        <v>108</v>
-      </c>
-      <c r="D34" s="16" t="s">
-        <v>18</v>
-      </c>
-      <c r="E34" s="16" t="s">
-        <v>19</v>
-      </c>
-      <c r="F34" s="17" t="n">
-        <v>1</v>
-      </c>
-      <c r="G34" s="17" t="n">
-        <v>0</v>
-      </c>
-      <c r="H34" s="17" t="n">
-        <v>0</v>
-      </c>
-      <c r="I34" s="13" t="n">
-        <v>0</v>
-      </c>
-      <c r="J34" s="16"/>
+      <c r="F34" s="12" t="n">
+        <v>1</v>
+      </c>
+      <c r="G34" s="12" t="n">
+        <v>0</v>
+      </c>
+      <c r="H34" s="12" t="n">
+        <v>0</v>
+      </c>
+      <c r="I34" s="12" t="n">
+        <v>0</v>
+      </c>
+      <c r="J34" s="15"/>
     </row>
     <row r="35" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A35" s="24" t="s">
-        <v>109</v>
-      </c>
-      <c r="B35" s="15" t="s">
+      <c r="A35" s="14" t="s">
         <v>110</v>
       </c>
-      <c r="C35" s="24" t="s">
+      <c r="B35" s="14" t="s">
         <v>111</v>
       </c>
-      <c r="D35" s="16" t="s">
-        <v>18</v>
-      </c>
-      <c r="E35" s="16" t="s">
-        <v>19</v>
-      </c>
-      <c r="F35" s="17" t="n">
-        <v>1</v>
-      </c>
-      <c r="G35" s="17" t="n">
-        <v>0</v>
-      </c>
-      <c r="H35" s="17" t="n">
-        <v>0</v>
-      </c>
-      <c r="I35" s="13" t="n">
-        <v>0</v>
-      </c>
-      <c r="J35" s="16"/>
+      <c r="C35" s="14" t="s">
+        <v>112</v>
+      </c>
+      <c r="D35" s="15" t="s">
+        <v>22</v>
+      </c>
+      <c r="E35" s="15" t="s">
+        <v>23</v>
+      </c>
+      <c r="F35" s="12" t="n">
+        <v>1</v>
+      </c>
+      <c r="G35" s="12" t="n">
+        <v>0</v>
+      </c>
+      <c r="H35" s="12" t="n">
+        <v>0</v>
+      </c>
+      <c r="I35" s="12" t="n">
+        <v>0</v>
+      </c>
+      <c r="J35" s="15"/>
     </row>
     <row r="36" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A36" s="15" t="s">
-        <v>112</v>
-      </c>
-      <c r="B36" s="15" t="s">
+      <c r="A36" s="20" t="s">
         <v>113</v>
       </c>
-      <c r="C36" s="15" t="s">
+      <c r="B36" s="14" t="s">
         <v>114</v>
       </c>
-      <c r="D36" s="16" t="s">
-        <v>18</v>
-      </c>
-      <c r="E36" s="16" t="s">
-        <v>19</v>
-      </c>
-      <c r="F36" s="17" t="n">
-        <v>1</v>
-      </c>
-      <c r="G36" s="17" t="n">
-        <v>0</v>
-      </c>
-      <c r="H36" s="17" t="n">
-        <v>0</v>
-      </c>
-      <c r="I36" s="13" t="n">
-        <v>0</v>
-      </c>
-      <c r="J36" s="16"/>
+      <c r="C36" s="20" t="s">
+        <v>115</v>
+      </c>
+      <c r="D36" s="15" t="s">
+        <v>22</v>
+      </c>
+      <c r="E36" s="15" t="s">
+        <v>23</v>
+      </c>
+      <c r="F36" s="12" t="n">
+        <v>1</v>
+      </c>
+      <c r="G36" s="12" t="n">
+        <v>0</v>
+      </c>
+      <c r="H36" s="12" t="n">
+        <v>0</v>
+      </c>
+      <c r="I36" s="12" t="n">
+        <v>0</v>
+      </c>
+      <c r="J36" s="15"/>
     </row>
     <row r="37" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A37" s="15" t="s">
-        <v>115</v>
-      </c>
-      <c r="B37" s="15" t="s">
+      <c r="A37" s="14" t="s">
         <v>116</v>
       </c>
-      <c r="C37" s="15" t="s">
+      <c r="B37" s="14" t="s">
         <v>117</v>
       </c>
-      <c r="D37" s="16" t="s">
-        <v>18</v>
-      </c>
-      <c r="E37" s="16"/>
-      <c r="F37" s="17" t="n">
-        <v>1</v>
-      </c>
-      <c r="G37" s="17" t="n">
-        <v>0</v>
-      </c>
-      <c r="H37" s="17" t="n">
-        <v>0</v>
-      </c>
-      <c r="I37" s="13" t="n">
-        <v>0</v>
-      </c>
-      <c r="J37" s="16"/>
+      <c r="C37" s="14" t="s">
+        <v>118</v>
+      </c>
+      <c r="D37" s="15" t="s">
+        <v>22</v>
+      </c>
+      <c r="E37" s="15" t="s">
+        <v>23</v>
+      </c>
+      <c r="F37" s="12" t="n">
+        <v>1</v>
+      </c>
+      <c r="G37" s="12" t="n">
+        <v>0</v>
+      </c>
+      <c r="H37" s="12" t="n">
+        <v>0</v>
+      </c>
+      <c r="I37" s="12" t="n">
+        <v>0</v>
+      </c>
+      <c r="J37" s="15"/>
     </row>
     <row r="38" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A38" s="15" t="s">
-        <v>118</v>
-      </c>
-      <c r="B38" s="15" t="s">
+      <c r="A38" s="14" t="s">
         <v>119</v>
       </c>
-      <c r="C38" s="15" t="s">
+      <c r="B38" s="14" t="s">
         <v>120</v>
       </c>
-      <c r="D38" s="16" t="s">
-        <v>18</v>
-      </c>
-      <c r="E38" s="16"/>
-      <c r="F38" s="17" t="n">
-        <v>1</v>
-      </c>
-      <c r="G38" s="17" t="n">
-        <v>0</v>
-      </c>
-      <c r="H38" s="17" t="n">
-        <v>0</v>
-      </c>
-      <c r="I38" s="13" t="n">
-        <v>0</v>
-      </c>
-      <c r="J38" s="16"/>
+      <c r="C38" s="14" t="s">
+        <v>121</v>
+      </c>
+      <c r="D38" s="15" t="s">
+        <v>22</v>
+      </c>
+      <c r="E38" s="15"/>
+      <c r="F38" s="12" t="n">
+        <v>1</v>
+      </c>
+      <c r="G38" s="12" t="n">
+        <v>0</v>
+      </c>
+      <c r="H38" s="12" t="n">
+        <v>0</v>
+      </c>
+      <c r="I38" s="12" t="n">
+        <v>0</v>
+      </c>
+      <c r="J38" s="15"/>
     </row>
     <row r="39" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A39" s="15" t="s">
-        <v>121</v>
-      </c>
-      <c r="B39" s="15" t="s">
+      <c r="A39" s="14" t="s">
         <v>122</v>
       </c>
-      <c r="C39" s="15" t="s">
+      <c r="B39" s="14" t="s">
         <v>123</v>
       </c>
-      <c r="D39" s="16" t="s">
-        <v>18</v>
-      </c>
-      <c r="E39" s="16"/>
-      <c r="F39" s="17" t="n">
-        <v>1</v>
-      </c>
-      <c r="G39" s="17" t="n">
-        <v>0</v>
-      </c>
-      <c r="H39" s="17" t="n">
-        <v>0</v>
-      </c>
-      <c r="I39" s="13" t="n">
-        <v>0</v>
-      </c>
-      <c r="J39" s="16"/>
-    </row>
-    <row r="40" customFormat="false" ht="30" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A40" s="15" t="s">
+      <c r="C39" s="14" t="s">
         <v>124</v>
       </c>
-      <c r="B40" s="15" t="s">
-        <v>122</v>
-      </c>
-      <c r="C40" s="15" t="s">
+      <c r="D39" s="15" t="s">
+        <v>22</v>
+      </c>
+      <c r="E39" s="15"/>
+      <c r="F39" s="12" t="n">
+        <v>1</v>
+      </c>
+      <c r="G39" s="12" t="n">
+        <v>0</v>
+      </c>
+      <c r="H39" s="12" t="n">
+        <v>0</v>
+      </c>
+      <c r="I39" s="12" t="n">
+        <v>0</v>
+      </c>
+      <c r="J39" s="15"/>
+    </row>
+    <row r="40" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A40" s="14" t="s">
         <v>125</v>
       </c>
-      <c r="D40" s="16" t="s">
-        <v>18</v>
-      </c>
-      <c r="E40" s="16"/>
-      <c r="F40" s="17" t="n">
-        <v>1</v>
-      </c>
-      <c r="G40" s="17" t="n">
-        <v>0</v>
-      </c>
-      <c r="H40" s="17" t="n">
-        <v>0</v>
-      </c>
-      <c r="I40" s="13" t="n">
-        <v>0</v>
-      </c>
-      <c r="J40" s="16"/>
+      <c r="B40" s="14" t="s">
+        <v>126</v>
+      </c>
+      <c r="C40" s="14" t="s">
+        <v>127</v>
+      </c>
+      <c r="D40" s="15" t="s">
+        <v>22</v>
+      </c>
+      <c r="E40" s="15"/>
+      <c r="F40" s="12" t="n">
+        <v>1</v>
+      </c>
+      <c r="G40" s="12" t="n">
+        <v>0</v>
+      </c>
+      <c r="H40" s="12" t="n">
+        <v>0</v>
+      </c>
+      <c r="I40" s="12" t="n">
+        <v>0</v>
+      </c>
+      <c r="J40" s="15"/>
     </row>
     <row r="41" customFormat="false" ht="30" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A41" s="15" t="s">
+      <c r="A41" s="14" t="s">
+        <v>128</v>
+      </c>
+      <c r="B41" s="14" t="s">
         <v>126</v>
       </c>
-      <c r="B41" s="15" t="s">
-        <v>127</v>
-      </c>
-      <c r="C41" s="15" t="s">
-        <v>128</v>
-      </c>
-      <c r="D41" s="16" t="s">
+      <c r="C41" s="14" t="s">
         <v>129</v>
       </c>
-      <c r="E41" s="16"/>
-      <c r="F41" s="17" t="n">
-        <v>1</v>
-      </c>
-      <c r="G41" s="17" t="n">
-        <v>0</v>
-      </c>
-      <c r="H41" s="17" t="n">
-        <v>0</v>
-      </c>
-      <c r="I41" s="13" t="n">
-        <v>0</v>
-      </c>
-      <c r="J41" s="16"/>
-    </row>
-    <row r="42" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A42" s="15" t="s">
+      <c r="D41" s="15" t="s">
+        <v>22</v>
+      </c>
+      <c r="E41" s="15"/>
+      <c r="F41" s="12" t="n">
+        <v>1</v>
+      </c>
+      <c r="G41" s="12" t="n">
+        <v>0</v>
+      </c>
+      <c r="H41" s="12" t="n">
+        <v>0</v>
+      </c>
+      <c r="I41" s="12" t="n">
+        <v>0</v>
+      </c>
+      <c r="J41" s="15"/>
+    </row>
+    <row r="42" customFormat="false" ht="30" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A42" s="14" t="s">
         <v>130</v>
       </c>
-      <c r="B42" s="15" t="s">
-        <v>127</v>
-      </c>
-      <c r="C42" s="15" t="s">
+      <c r="B42" s="14" t="s">
         <v>131</v>
       </c>
-      <c r="D42" s="16" t="s">
-        <v>129</v>
-      </c>
-      <c r="E42" s="16"/>
-      <c r="F42" s="17" t="n">
-        <v>1</v>
-      </c>
-      <c r="G42" s="17" t="n">
-        <v>0</v>
-      </c>
-      <c r="H42" s="17" t="n">
-        <v>0</v>
-      </c>
-      <c r="I42" s="13" t="n">
-        <v>0</v>
-      </c>
-      <c r="J42" s="16"/>
+      <c r="C42" s="14" t="s">
+        <v>132</v>
+      </c>
+      <c r="D42" s="15" t="s">
+        <v>133</v>
+      </c>
+      <c r="E42" s="15"/>
+      <c r="F42" s="12" t="n">
+        <v>1</v>
+      </c>
+      <c r="G42" s="12" t="n">
+        <v>0</v>
+      </c>
+      <c r="H42" s="12" t="n">
+        <v>0</v>
+      </c>
+      <c r="I42" s="12" t="n">
+        <v>0</v>
+      </c>
+      <c r="J42" s="15"/>
     </row>
     <row r="43" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A43" s="15" t="s">
-        <v>132</v>
-      </c>
-      <c r="B43" s="15" t="s">
-        <v>127</v>
-      </c>
-      <c r="C43" s="15" t="s">
+      <c r="A43" s="14" t="s">
+        <v>134</v>
+      </c>
+      <c r="B43" s="14" t="s">
+        <v>131</v>
+      </c>
+      <c r="C43" s="14" t="s">
+        <v>135</v>
+      </c>
+      <c r="D43" s="15" t="s">
         <v>133</v>
       </c>
-      <c r="D43" s="16" t="s">
-        <v>129</v>
-      </c>
-      <c r="E43" s="16"/>
-      <c r="F43" s="17" t="n">
-        <v>1</v>
-      </c>
-      <c r="G43" s="17" t="n">
-        <v>0</v>
-      </c>
-      <c r="H43" s="17" t="n">
-        <v>0</v>
-      </c>
-      <c r="I43" s="13" t="n">
-        <v>0</v>
-      </c>
-      <c r="J43" s="16"/>
+      <c r="E43" s="15"/>
+      <c r="F43" s="12" t="n">
+        <v>1</v>
+      </c>
+      <c r="G43" s="12" t="n">
+        <v>0</v>
+      </c>
+      <c r="H43" s="12" t="n">
+        <v>0</v>
+      </c>
+      <c r="I43" s="12" t="n">
+        <v>0</v>
+      </c>
+      <c r="J43" s="15"/>
     </row>
     <row r="44" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A44" s="15" t="s">
-        <v>134</v>
-      </c>
-      <c r="B44" s="15" t="s">
-        <v>127</v>
-      </c>
-      <c r="C44" s="15" t="s">
+      <c r="A44" s="14" t="s">
+        <v>136</v>
+      </c>
+      <c r="B44" s="14" t="s">
+        <v>131</v>
+      </c>
+      <c r="C44" s="14" t="s">
+        <v>137</v>
+      </c>
+      <c r="D44" s="15" t="s">
         <v>133</v>
       </c>
-      <c r="D44" s="16" t="s">
-        <v>129</v>
-      </c>
-      <c r="E44" s="16"/>
-      <c r="F44" s="17" t="n">
-        <v>1</v>
-      </c>
-      <c r="G44" s="17" t="n">
-        <v>0</v>
-      </c>
-      <c r="H44" s="17" t="n">
-        <v>0</v>
-      </c>
-      <c r="I44" s="13" t="n">
-        <v>0</v>
-      </c>
-      <c r="J44" s="16"/>
+      <c r="E44" s="15"/>
+      <c r="F44" s="12" t="n">
+        <v>1</v>
+      </c>
+      <c r="G44" s="12" t="n">
+        <v>0</v>
+      </c>
+      <c r="H44" s="12" t="n">
+        <v>0</v>
+      </c>
+      <c r="I44" s="12" t="n">
+        <v>0</v>
+      </c>
+      <c r="J44" s="15"/>
+    </row>
+    <row r="45" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A45" s="14" t="s">
+        <v>138</v>
+      </c>
+      <c r="B45" s="14" t="s">
+        <v>131</v>
+      </c>
+      <c r="C45" s="14" t="s">
+        <v>137</v>
+      </c>
+      <c r="D45" s="15" t="s">
+        <v>133</v>
+      </c>
+      <c r="E45" s="15"/>
+      <c r="F45" s="12" t="n">
+        <v>1</v>
+      </c>
+      <c r="G45" s="12" t="n">
+        <v>0</v>
+      </c>
+      <c r="H45" s="12" t="n">
+        <v>0</v>
+      </c>
+      <c r="I45" s="12" t="n">
+        <v>0</v>
+      </c>
+      <c r="J45" s="15"/>
     </row>
   </sheetData>
   <mergeCells count="1">
     <mergeCell ref="A1:E1"/>
   </mergeCells>
-  <conditionalFormatting sqref="F3:I741">
+  <conditionalFormatting sqref="F5:I742,F3:I3">
     <cfRule type="cellIs" priority="2" operator="equal" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="0">
       <formula>1</formula>
     </cfRule>
@@ -3151,8 +3173,16 @@
       <formula>1</formula>
     </cfRule>
   </conditionalFormatting>
+  <conditionalFormatting sqref="F4:I4">
+    <cfRule type="cellIs" priority="5" operator="equal" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="0">
+      <formula>1</formula>
+    </cfRule>
+    <cfRule type="cellIs" priority="6" operator="equal" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="1">
+      <formula>0</formula>
+    </cfRule>
+  </conditionalFormatting>
   <dataValidations count="1">
-    <dataValidation allowBlank="true" operator="between" showDropDown="false" showErrorMessage="true" showInputMessage="true" sqref="F3:I44" type="whole">
+    <dataValidation allowBlank="true" operator="between" showDropDown="false" showErrorMessage="true" showInputMessage="true" sqref="F3:I45" type="whole">
       <formula1>0</formula1>
       <formula2>1</formula2>
     </dataValidation>

</xml_diff>

<commit_message>
ASKAPSDP-2214 work in progress on polarisation data ingest
</commit_message>
<xml_diff>
--- a/Code/Components/Services/skymodel/current/schema_definitions/GSM_casda_polarisation.xlsx
+++ b/Code/Components/Services/skymodel/current/schema_definitions/GSM_casda_polarisation.xlsx
@@ -702,7 +702,7 @@
     <cellStyle name="Currency" xfId="17" builtinId="4" customBuiltin="false"/>
     <cellStyle name="Currency [0]" xfId="18" builtinId="7" customBuiltin="false"/>
     <cellStyle name="Percent" xfId="19" builtinId="5" customBuiltin="false"/>
-    <cellStyle name="Excel Built-in Excel Built-in Neutral" xfId="20" builtinId="54" customBuiltin="true"/>
+    <cellStyle name="Excel Built-in Excel Built-in Excel Built-in Neutral" xfId="20" builtinId="54" customBuiltin="true"/>
   </cellStyles>
   <dxfs count="3">
     <dxf>
@@ -818,8 +818,8 @@
   </sheetPr>
   <dimension ref="1:45"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A4" activeCellId="0" sqref="A4"/>
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A22" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="D45" activeCellId="0" sqref="D45"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.95"/>
@@ -3160,24 +3160,16 @@
   <mergeCells count="1">
     <mergeCell ref="A1:E1"/>
   </mergeCells>
-  <conditionalFormatting sqref="F5:I742,F3:I3">
-    <cfRule type="cellIs" priority="2" operator="equal" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="0">
-      <formula>1</formula>
-    </cfRule>
-    <cfRule type="cellIs" priority="3" operator="equal" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="1">
-      <formula>0</formula>
-    </cfRule>
-  </conditionalFormatting>
   <conditionalFormatting sqref="F2:I2">
-    <cfRule type="cellIs" priority="4" operator="equal" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="2">
+    <cfRule type="cellIs" priority="2" operator="equal" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="2">
       <formula>1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="F4:I4">
-    <cfRule type="cellIs" priority="5" operator="equal" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="0">
+    <cfRule type="cellIs" priority="3" operator="equal" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="0">
       <formula>1</formula>
     </cfRule>
-    <cfRule type="cellIs" priority="6" operator="equal" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="1">
+    <cfRule type="cellIs" priority="4" operator="equal" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="1">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>

</xml_diff>